<commit_message>
tranferred o2 and alk data from rr18045 drive on data camo
</commit_message>
<xml_diff>
--- a/data/flux/rates/alk-calk.xlsx
+++ b/data/flux/rates/alk-calk.xlsx
@@ -196,7 +196,7 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
+      <selection pane="topLeft" activeCell="Q7" activeCellId="0" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -345,26 +345,34 @@
         <v>2750</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>7.598</v>
+        <v>7.611</v>
       </c>
       <c r="J3" s="1" t="n">
         <v>7.572</v>
       </c>
       <c r="K3" s="1" t="n">
-        <v>34.7</v>
+        <v>34.5183</v>
       </c>
       <c r="L3" s="1" t="n">
-        <v>11.7321</v>
-      </c>
-      <c r="M3" s="1"/>
+        <v>10.9108</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <v>191.321</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>150.448</v>
+      </c>
       <c r="O3" s="1" t="n">
-        <v>23.88</v>
+        <v>29.7</v>
       </c>
       <c r="P3" s="1" t="n">
-        <v>2.41</v>
+        <v>2.54</v>
       </c>
       <c r="Q3" s="1" t="n">
         <v>7.2</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <v>2.71</v>
       </c>
       <c r="S3" s="0" t="n">
         <v>2.47</v>

</xml_diff>

<commit_message>
input i think real 120 m p1 2018 alks
</commit_message>
<xml_diff>
--- a/data/flux/rates/alk-calk.xlsx
+++ b/data/flux/rates/alk-calk.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -79,13 +79,19 @@
     <t xml:space="preserve">ctd dic</t>
   </si>
   <si>
+    <t xml:space="preserve">plus p rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ctl rate</t>
+  </si>
+  <si>
     <t xml:space="preserve">p1</t>
   </si>
   <si>
     <t xml:space="preserve">cone</t>
   </si>
   <si>
-    <t xml:space="preserve">post p alk needs to be checked, right now my old values and I’m not sure where they’re from</t>
+    <t xml:space="preserve">post p alk for 2018 p1 120 180 needs to be checked, right now my old values and I’m not sure where they’re from</t>
   </si>
   <si>
     <t xml:space="preserve">other ctd and ctl alks from POMZ/Keil/Alk/Alk_rawdata</t>
@@ -103,6 +109,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -123,6 +130,7 @@
       <sz val="10"/>
       <name val="Courier New"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -167,8 +175,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -193,199 +205,221 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q7" activeCellId="0" sqref="Q7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q3" activeCellId="0" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>2018</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="0" t="n">
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>2506</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="G2" s="2" t="n">
         <v>2583</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="2" t="n">
         <v>2622</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="1" t="n">
         <v>7.598</v>
       </c>
-      <c r="J2" s="1" t="n">
+      <c r="J2" s="2" t="n">
         <v>7.572</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2" s="1" t="n">
         <v>34.8144</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="L2" s="1" t="n">
         <v>12.9378</v>
       </c>
-      <c r="M2" s="1" t="n">
+      <c r="M2" s="2" t="n">
         <v>120.814</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="N2" s="1" t="n">
         <v>125.625</v>
       </c>
-      <c r="O2" s="0" t="n">
+      <c r="O2" s="1" t="n">
         <v>27.04</v>
       </c>
-      <c r="P2" s="0" t="n">
+      <c r="P2" s="1" t="n">
         <v>2.51</v>
       </c>
-      <c r="Q2" s="0" t="n">
-        <v>7.22</v>
-      </c>
-      <c r="R2" s="0" t="n">
+      <c r="Q2" s="1" t="n">
+        <v>2.56</v>
+      </c>
+      <c r="R2" s="1" t="n">
         <v>2.59</v>
       </c>
-      <c r="S2" s="0" t="n">
+      <c r="S2" s="1" t="n">
         <v>2.46</v>
+      </c>
+      <c r="T2" s="0" t="n">
+        <f aca="false">Q2-S2/(E2/24)</f>
+        <v>-0.392</v>
+      </c>
+      <c r="U2" s="0" t="n">
+        <f aca="false">R2-S2/(E2/24)</f>
+        <v>-0.362</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2018</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="0" t="n">
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="n">
         <v>190</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>2503</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>2589</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="1" t="n">
         <v>2750</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="1" t="n">
         <v>7.611</v>
       </c>
-      <c r="J3" s="1" t="n">
+      <c r="J3" s="2" t="n">
         <v>7.572</v>
       </c>
-      <c r="K3" s="1" t="n">
+      <c r="K3" s="2" t="n">
         <v>34.5183</v>
       </c>
-      <c r="L3" s="1" t="n">
+      <c r="L3" s="2" t="n">
         <v>10.9108</v>
       </c>
-      <c r="M3" s="1" t="n">
+      <c r="M3" s="2" t="n">
         <v>191.321</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="N3" s="1" t="n">
         <v>150.448</v>
       </c>
-      <c r="O3" s="1" t="n">
+      <c r="O3" s="2" t="n">
         <v>29.7</v>
       </c>
-      <c r="P3" s="1" t="n">
+      <c r="P3" s="2" t="n">
         <v>2.54</v>
       </c>
-      <c r="Q3" s="1" t="n">
+      <c r="Q3" s="2" t="n">
         <v>7.2</v>
       </c>
-      <c r="R3" s="0" t="n">
+      <c r="R3" s="1" t="n">
         <v>2.71</v>
       </c>
-      <c r="S3" s="0" t="n">
+      <c r="S3" s="1" t="n">
         <v>2.47</v>
       </c>
+      <c r="T3" s="0" t="n">
+        <f aca="false">Q3-S3/(E3/24)</f>
+        <v>4.236</v>
+      </c>
+      <c r="U3" s="0" t="n">
+        <f aca="false">R3-S3/(E3/24)</f>
+        <v>-0.254</v>
+      </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>21</v>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>22</v>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed 1200 and 100 p2 ctd alk cald dic
</commit_message>
<xml_diff>
--- a/data/flux/rates/alk-calk.xlsx
+++ b/data/flux/rates/alk-calk.xlsx
@@ -20,91 +20,87 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
-  <si>
-    <t xml:space="preserve">year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">station</t>
-  </si>
-  <si>
-    <t xml:space="preserve">depth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">trap type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inc time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ctd alk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">post p alk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">post ctl alk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ctd ph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inc ph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ctd salinity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ctd temp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">trap pressure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ctd pressure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">silicate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phosphate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">post p dic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">post ctl dic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ctd dic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plus p rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ctl rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+  <si>
+    <t xml:space="preserve">Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Station</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trap type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incubation time (hr)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niskin alk (umol)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post plus P alk (umol)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post Ctl alk (umol)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niskin pH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incubator pH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD salinity (PSU)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD temp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incubator pressure (dbar)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD pressure (dbar)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silicate (umol)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phosphate (umol)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post plus P DIC (mmol)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post Ctl DIC (mmol)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niskin DIC (mmol)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plus P rate (mmol C/day)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ctl rate (mmol C/day)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P1</t>
   </si>
   <si>
     <t xml:space="preserve">cone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">post p alk for 2018 p1 120 180 needs to be checked, right now my old values and I’m not sure where they’re from</t>
-  </si>
-  <si>
-    <t xml:space="preserve">other ctd and ctl alks from POMZ/Keil/Alk/Alk_rawdata</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -125,12 +121,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -175,7 +165,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -184,7 +174,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -205,13 +211,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U22"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q3" activeCellId="0" sqref="Q3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="1" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="11.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="11.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="18" style="1" width="11.56"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -256,13 +269,13 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
@@ -271,10 +284,10 @@
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -297,16 +310,16 @@
       <c r="F2" s="1" t="n">
         <v>2506</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="4" t="n">
         <v>2583</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="H2" s="4" t="n">
         <v>2622</v>
       </c>
       <c r="I2" s="1" t="n">
         <v>7.598</v>
       </c>
-      <c r="J2" s="2" t="n">
+      <c r="J2" s="4" t="n">
         <v>7.572</v>
       </c>
       <c r="K2" s="1" t="n">
@@ -315,19 +328,19 @@
       <c r="L2" s="1" t="n">
         <v>12.9378</v>
       </c>
-      <c r="M2" s="2" t="n">
+      <c r="M2" s="4" t="n">
         <v>120.814</v>
       </c>
       <c r="N2" s="1" t="n">
         <v>125.625</v>
       </c>
-      <c r="O2" s="1" t="n">
+      <c r="O2" s="2" t="n">
         <v>27.04</v>
       </c>
       <c r="P2" s="1" t="n">
         <v>2.51</v>
       </c>
-      <c r="Q2" s="1" t="n">
+      <c r="Q2" s="3" t="n">
         <v>2.56</v>
       </c>
       <c r="R2" s="1" t="n">
@@ -336,11 +349,11 @@
       <c r="S2" s="1" t="n">
         <v>2.46</v>
       </c>
-      <c r="T2" s="0" t="n">
+      <c r="T2" s="1" t="n">
         <f aca="false">Q2-S2/(E2/24)</f>
         <v>-0.392</v>
       </c>
-      <c r="U2" s="0" t="n">
+      <c r="U2" s="1" t="n">
         <f aca="false">R2-S2/(E2/24)</f>
         <v>-0.362</v>
       </c>
@@ -373,28 +386,28 @@
       <c r="I3" s="1" t="n">
         <v>7.611</v>
       </c>
-      <c r="J3" s="2" t="n">
+      <c r="J3" s="4" t="n">
         <v>7.572</v>
       </c>
-      <c r="K3" s="2" t="n">
+      <c r="K3" s="4" t="n">
         <v>34.5183</v>
       </c>
-      <c r="L3" s="2" t="n">
+      <c r="L3" s="4" t="n">
         <v>10.9108</v>
       </c>
-      <c r="M3" s="2" t="n">
+      <c r="M3" s="4" t="n">
         <v>191.321</v>
       </c>
       <c r="N3" s="1" t="n">
         <v>150.448</v>
       </c>
-      <c r="O3" s="2" t="n">
+      <c r="O3" s="5" t="n">
         <v>29.7</v>
       </c>
-      <c r="P3" s="2" t="n">
+      <c r="P3" s="4" t="n">
         <v>2.54</v>
       </c>
-      <c r="Q3" s="2" t="n">
+      <c r="Q3" s="6" t="n">
         <v>7.2</v>
       </c>
       <c r="R3" s="1" t="n">
@@ -403,23 +416,13 @@
       <c r="S3" s="1" t="n">
         <v>2.47</v>
       </c>
-      <c r="T3" s="0" t="n">
+      <c r="T3" s="1" t="n">
         <f aca="false">Q3-S3/(E3/24)</f>
         <v>4.236</v>
       </c>
-      <c r="U3" s="0" t="n">
+      <c r="U3" s="1" t="n">
         <f aca="false">R3-S3/(E3/24)</f>
         <v>-0.254</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>